<commit_message>
had to make a change to the code
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Especializado/Data/CCNayarTemplate_Especializado_1.1.xlsx
+++ b/Projects/CCNAYARMX/Especializado/Data/CCNayarTemplate_Especializado_1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,6 +62,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2017,23 +2020,23 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.3441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="68.8785425101215"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="131.542510121458"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8461538461538"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="135.076923076923"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="11" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
@@ -2071,7 +2074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="true" ht="61.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="7" customFormat="true" ht="61.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -2176,7 +2179,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="125" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="125" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>11</v>
       </c>
@@ -2680,7 +2683,7 @@
       </c>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
         <v>25</v>
       </c>
@@ -2708,7 +2711,7 @@
       </c>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="39" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>21</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="n">
         <v>27</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
         <v>37</v>
       </c>
@@ -3538,7 +3541,7 @@
       <c r="I58" s="26"/>
       <c r="J58" s="22"/>
     </row>
-    <row r="59" customFormat="false" ht="32.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="n">
         <v>42</v>
       </c>
@@ -3666,7 +3669,7 @@
       <c r="I63" s="26"/>
       <c r="J63" s="22"/>
     </row>
-    <row r="64" customFormat="false" ht="32" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="n">
         <v>47</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <v>51</v>
       </c>
@@ -3796,7 +3799,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <v>52</v>
       </c>
@@ -3819,10 +3822,12 @@
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:J69">
-    <filterColumn colId="6">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Scoring"/>
-      </customFilters>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Plataformas-Especializado"/>
+        <filter val="La plataforma esta libre de objetos diferentes al portafolio valido-Hidratacion?-Especializado"/>
+        <filter val="La plataforma esta libre de objetos diferentes al portafolio valido-Nutricion?-Especializado"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">
@@ -3853,11 +3858,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7125506072875"/>
@@ -3979,18 +3984,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="54" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="66.8421052631579"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="95.6558704453441"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="54" width="66.8421052631579"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="99.2995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="54" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="68.5546558704453"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="98.2267206477733"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="54" width="68.5546558704453"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="101.975708502024"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="74.3400809716599"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="54" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="54" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="54" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="54" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="54" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="54" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="54" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="54" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="54" width="11.6761133603239"/>
@@ -4405,22 +4410,22 @@
   </sheetPr>
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="115.902834008097"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="77.7692307692308"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="119.008097165992"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
@@ -4809,7 +4814,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="N58" activeCellId="0" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4936,13 +4941,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.0971659919028"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="58.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
@@ -5058,19 +5063,19 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.9514170040486"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="68.8785425101215"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="0" width="9.10526315789474"/>
@@ -5243,21 +5248,21 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="85.3724696356275"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="87.6234817813765"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.8421052631579"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.2753036437247"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.3481781376518"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="47.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5546558704453"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="48.8461538461539"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -5598,14 +5603,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="40.2753036437247"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
@@ -5728,18 +5733,18 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.9838056680162"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.8785425101215"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="179.21052631579"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.5910931174089"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="184.137651821862"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -5947,21 +5952,21 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="54" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="62.8785425101215"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="77.7692307692308"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="64.5910931174089"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="84.6234817813765"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="54" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="54" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="105.51012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="54" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="108.404858299595"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="54" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="54" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="54" width="13.3886639676113"/>
@@ -6444,20 +6449,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="66.8421052631579"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="95.6558704453441"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="51.417004048583"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.7732793522267"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="68.5546558704453"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="98.2267206477733"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
@@ -6671,19 +6676,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.7327935222672"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="71.4493927125506"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10526315789474"/>
   </cols>
@@ -6871,18 +6876,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.2712550607288"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.8785425101215"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7024,7 +7029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="77" t="n">
         <v>45</v>
       </c>
@@ -7038,7 +7043,7 @@
         <v>146</v>
       </c>
       <c r="E7" s="74" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="75" t="s">
         <v>253</v>
@@ -7047,7 +7052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="76" t="n">
         <v>46</v>
       </c>
@@ -7061,7 +7066,7 @@
         <v>146</v>
       </c>
       <c r="E8" s="74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F8" s="75" t="s">
         <v>254</v>
@@ -7114,6 +7119,9 @@
       <c r="H10" s="7"/>
       <c r="I10" s="35"/>
       <c r="J10" s="60"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Corrected the changes in the template
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Especializado/Data/CCNayarTemplate_Especializado_1.1.xlsx
+++ b/Projects/CCNAYARMX/Especializado/Data/CCNayarTemplate_Especializado_1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -65,6 +65,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$69</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1220,7 +1221,7 @@
     <t xml:space="preserve">Product sub_category</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Facings Target</t>
+    <t xml:space="preserve">Unique Products Targets</t>
   </si>
   <si>
     <t xml:space="preserve">numerator_entity</t>
@@ -2023,20 +2024,20 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
+      <selection pane="bottomLeft" activeCell="D64" activeCellId="1" sqref="K1 D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8461538461538"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="135.076923076923"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="136.36032388664"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="11" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
@@ -3852,17 +3853,17 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="K1 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7125506072875"/>
@@ -3979,23 +3980,23 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="K1 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="54" width="63.9514170040486"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="98.2267206477733"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="54" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="101.975708502024"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="54" width="64.5910931174089"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="99.085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="54" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="102.939271255061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="74.9838056680162"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="54" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="54" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="54" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="54" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="54" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="54" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="54" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="54" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="54" width="11.6761133603239"/>
@@ -4410,22 +4411,22 @@
   </sheetPr>
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="K1 C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.6356275303644"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="119.008097165992"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="79.8016194331984"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="120.080971659919"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="80.4453441295547"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
@@ -4814,7 +4815,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N58" activeCellId="0" sqref="N58"/>
+      <selection pane="topLeft" activeCell="N58" activeCellId="1" sqref="K1 N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4934,24 +4935,24 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.5263157894737"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="59.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="27.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -5064,18 +5065,18 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="K1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.4858299595142"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="0" width="9.10526315789474"/>
@@ -5242,27 +5243,27 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="K1 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="88.4817813765182"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.5587044534413"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="49.2753036437247"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -5592,7 +5593,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="K1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5603,14 +5604,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
@@ -5734,17 +5735,17 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="K1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.7327935222672"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.5910931174089"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="184.137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.1295546558705"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="185.744939271255"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -5953,20 +5954,20 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="K1 J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="54" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="64.5910931174089"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="79.8016194331984"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="84.6234817813765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="65.1295546558705"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="80.4453441295547"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="54" width="85.3724696356275"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="54" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="54" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="108.404858299595"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="54" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="109.368421052632"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="54" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="54" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="54" width="13.3886639676113"/>
@@ -6443,26 +6444,26 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="K1 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="63.9514170040486"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.7732793522267"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="98.2267206477733"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="52.7044534412956"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="64.5910931174089"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.3076923076923"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="99.085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="53.1295546558704"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.9554655870445"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
@@ -6671,24 +6672,24 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="K1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10526315789474"/>
   </cols>
@@ -6879,15 +6880,15 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="1" sqref="K1 E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.8785425101215"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="69.5182186234818"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>